<commit_message>
update README and JSON_comparison
</commit_message>
<xml_diff>
--- a/JSON_comparison.xlsx
+++ b/JSON_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smalldragon/code/grpc/transfer-df/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF33D3E-0F7C-6843-868B-514A0418531C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F22F12-9236-CE47-973E-ED25E2381494}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{9F4D194F-1635-C94D-9D93-F8DB2AEE1290}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{9F4D194F-1635-C94D-9D93-F8DB2AEE1290}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -255,44 +255,6 @@
         <charset val="136"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="176" formatCode="0.0000"/>
     </dxf>
     <dxf>
@@ -310,76 +272,6 @@
         <color theme="1"/>
         <name val="新細明體"/>
         <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="176" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="176" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="176" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="新細明體"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="176" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="新細明體"/>
         <charset val="136"/>
         <scheme val="minor"/>
       </font>
@@ -500,6 +392,114 @@
         <color theme="1"/>
         <name val="新細明體"/>
         <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="176" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="176" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="176" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="新細明體"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="176" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="新細明體"/>
         <charset val="136"/>
         <scheme val="minor"/>
       </font>
@@ -644,11 +644,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$B$2</c:f>
+              <c:f>工作表1!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> total_mean</c:v>
+                  <c:v>Non Compat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -816,104 +816,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$E$2</c:f>
+              <c:f>工作表1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>method</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>工作表1!$A$3:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>GetRowJSON</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>GetRowuJSON</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>GetRoworJSON</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>GetChunkedJSON</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>GetChunkeduJSON</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GetChunkedorJSON</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>GetColumnJSON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>工作表1!$E$3:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-D445-2540-A25E-503D8B916D7D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>工作表1!$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v> total_mean</c:v>
+                  <c:v>Compat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1121,6 +1032,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1251,11 +1193,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$B$13</c:f>
+              <c:f>工作表1!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> total_mean</c:v>
+                  <c:v>Non Compat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1336,104 +1278,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$E$13</c:f>
+              <c:f>工作表1!$E$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>method</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>工作表1!$A$14:$A$20</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>GetRowJSON</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>GetRowuJSON</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>GetRoworJSON</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>GetChunkedJSON</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>GetChunkeduJSON</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GetChunkedorJSON</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>GetColumnJSON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>工作表1!$E$14:$E$20</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-84F9-0246-8A83-5B44EE61DBEB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>工作表1!$F$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v> total_mean</c:v>
+                  <c:v>Compat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1641,6 +1494,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2855,30 +2739,30 @@
   <autoFilter ref="A2:C9" xr:uid="{6A97BD64-6C14-9540-9B39-DDA275A68A90}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{3E6E950D-A506-E74B-ACF8-828DCAD6C4B5}" name="method" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{383D0824-F5B5-FB40-9002-A95C0B8C6F45}" name=" total_mean" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{4D0225A1-3F18-1940-84DE-808F565CE84D}" name=" total_std" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{383D0824-F5B5-FB40-9002-A95C0B8C6F45}" name=" total_mean" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{4D0225A1-3F18-1940-84DE-808F565CE84D}" name=" total_std" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1882EC19-B3C9-2746-94C1-901E62D610BB}" name="表格2" displayName="表格2" ref="E2:G9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1882EC19-B3C9-2746-94C1-901E62D610BB}" name="表格2" displayName="表格2" ref="E2:G9" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="E2:G9" xr:uid="{2943088A-2028-D94D-9DF6-3F9319D6A26C}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C262073F-A3ED-2B41-BB74-77B644D71133}" name="method" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{A9907975-BE60-6043-BDEA-11CE54DC2881}" name=" total_mean" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{CD4B245A-536D-A041-A608-FF4E865E4ACA}" name=" total_std" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C262073F-A3ED-2B41-BB74-77B644D71133}" name="method" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{A9907975-BE60-6043-BDEA-11CE54DC2881}" name=" total_mean" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{CD4B245A-536D-A041-A608-FF4E865E4ACA}" name=" total_std" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EDEFE7A3-17B0-0548-804F-4EBC0EB06D2B}" name="表格3" displayName="表格3" ref="E13:G20" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EDEFE7A3-17B0-0548-804F-4EBC0EB06D2B}" name="表格3" displayName="表格3" ref="E13:G20" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="E13:G20" xr:uid="{E71390ED-608A-B740-9054-A68593E1C738}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3334A3EF-8917-AB43-88F0-B75E8C2383A9}" name="method" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{3334A3EF-8917-AB43-88F0-B75E8C2383A9}" name="method" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{F3EDA41E-EEC6-5E42-BA9F-E80B953F84B2}" name=" total_mean" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{B988A898-2325-4142-B909-17F991CCA6E4}" name=" total_std" dataDxfId="5"/>
   </tableColumns>
@@ -2887,12 +2771,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AE63CF7D-84DF-6C44-B762-2A46F78E5811}" name="表格4" displayName="表格4" ref="A13:C20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AE63CF7D-84DF-6C44-B762-2A46F78E5811}" name="表格4" displayName="表格4" ref="A13:C20" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A13:C20" xr:uid="{8EA6B4ED-A029-A34E-BF86-B966840DA656}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2818AF58-9ABC-FB49-B22D-E5A89A900380}" name="method" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{7868007B-819D-AE42-87C7-FE23172E0FD4}" name=" total_mean" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{1459305E-F8E2-9B49-8F35-E42A6793F641}" name=" total_std" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{2818AF58-9ABC-FB49-B22D-E5A89A900380}" name="method" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{7868007B-819D-AE42-87C7-FE23172E0FD4}" name=" total_mean" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{1459305E-F8E2-9B49-8F35-E42A6793F641}" name=" total_std" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3197,8 +3081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61033DBB-B72A-9344-9BB6-90B3CC73F8CB}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>

</xml_diff>